<commit_message>
Comenzando con Random Forest
</commit_message>
<xml_diff>
--- a/ComparativaModelos.xlsx
+++ b/ComparativaModelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/UCM/Machine Learning/Practica ML/MachineLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB5400A-1B09-B541-ADD1-B1E6B9FC7C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A03A3-A38B-224F-8967-83B8D2F199FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="avnnet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="120">
   <si>
     <t>tasa</t>
   </si>
@@ -278,6 +278,123 @@
   </si>
   <si>
     <t>AVNNET MODELO 2</t>
+  </si>
+  <si>
+    <t>0.10112743</t>
+  </si>
+  <si>
+    <t>0.9126257</t>
+  </si>
+  <si>
+    <t>0.09993167</t>
+  </si>
+  <si>
+    <t>0.9144836</t>
+  </si>
+  <si>
+    <t>0.09890673</t>
+  </si>
+  <si>
+    <t>0.9145415</t>
+  </si>
+  <si>
+    <t>0.09959002</t>
+  </si>
+  <si>
+    <t>0.9140330</t>
+  </si>
+  <si>
+    <t>0.10027332</t>
+  </si>
+  <si>
+    <t>0.9140948</t>
+  </si>
+  <si>
+    <t>0.09941920</t>
+  </si>
+  <si>
+    <t>0.9147203</t>
+  </si>
+  <si>
+    <t>0.10010249</t>
+  </si>
+  <si>
+    <t>0.9145659</t>
+  </si>
+  <si>
+    <t>0.09907755</t>
+  </si>
+  <si>
+    <t>0.9155725</t>
+  </si>
+  <si>
+    <t>0.10095661</t>
+  </si>
+  <si>
+    <t>0.9155204</t>
+  </si>
+  <si>
+    <t>0.9127317</t>
+  </si>
+  <si>
+    <t>BAG. MODELO 2</t>
+  </si>
+  <si>
+    <t>0.10181073</t>
+  </si>
+  <si>
+    <t>0.9124968</t>
+  </si>
+  <si>
+    <t>0.10317731</t>
+  </si>
+  <si>
+    <t>0.9144305</t>
+  </si>
+  <si>
+    <t>0.10078579</t>
+  </si>
+  <si>
+    <t>0.9143850</t>
+  </si>
+  <si>
+    <t>0.9138405</t>
+  </si>
+  <si>
+    <t>0.10198155</t>
+  </si>
+  <si>
+    <t>0.9144000</t>
+  </si>
+  <si>
+    <t>0.10061496</t>
+  </si>
+  <si>
+    <t>0.9151003</t>
+  </si>
+  <si>
+    <t>0.10249402</t>
+  </si>
+  <si>
+    <t>0.9151371</t>
+  </si>
+  <si>
+    <t>0.10163990</t>
+  </si>
+  <si>
+    <t>0.9150177</t>
+  </si>
+  <si>
+    <t>0.10129826</t>
+  </si>
+  <si>
+    <t>0.9149272</t>
+  </si>
+  <si>
+    <t>0.9136212</t>
+  </si>
+  <si>
+    <t>BAG. MODELO 1</t>
   </si>
 </sst>
 </file>
@@ -637,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD02A42-AD32-D845-B847-33E6CA93CE32}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:C41"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C725FB-0259-044F-8EEE-299F54C2EEBC}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="C41" sqref="A22:C41"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,6 +1461,446 @@
         <v>40</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59" t="s">
+        <v>96</v>
+      </c>
+      <c r="C59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Comenzando con gradient boosting...
</commit_message>
<xml_diff>
--- a/ComparativaModelos.xlsx
+++ b/ComparativaModelos.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/UCM/Machine Learning/Practica ML/MachineLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD291F7-DE50-A34D-A414-190725E80825}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5711DF70-C315-F04A-94F2-B96EE5B4EB9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" activeTab="1" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="2" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="avnnet" sheetId="1" r:id="rId1"/>
     <sheet name="bagging" sheetId="2" r:id="rId2"/>
+    <sheet name="random_forest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="153">
   <si>
     <t>tasa</t>
   </si>
@@ -115,9 +116,6 @@
     <t>BAG. MODELO 2</t>
   </si>
   <si>
-    <t>0.10317731</t>
-  </si>
-  <si>
     <t>BAG. MODELO 1</t>
   </si>
   <si>
@@ -286,119 +284,224 @@
     <t>0.8879191</t>
   </si>
   <si>
-    <t>0.10830202</t>
-  </si>
-  <si>
-    <t>0.9124821</t>
+    <t>0.10454390</t>
+  </si>
+  <si>
+    <t>0.10522720</t>
+  </si>
+  <si>
+    <t>0.10659378</t>
+  </si>
+  <si>
+    <t>RF. MODELO 1</t>
+  </si>
+  <si>
+    <t>0.10591049</t>
+  </si>
+  <si>
+    <t>RF. MODELO 2</t>
+  </si>
+  <si>
+    <t>0.10215237</t>
+  </si>
+  <si>
+    <t>0.10078579</t>
+  </si>
+  <si>
+    <t>0.10181073</t>
+  </si>
+  <si>
+    <t>0.10027332</t>
+  </si>
+  <si>
+    <t>0.09993167</t>
+  </si>
+  <si>
+    <t>0.10061496</t>
+  </si>
+  <si>
+    <t>0.10129826</t>
+  </si>
+  <si>
+    <t>0.10163990</t>
+  </si>
+  <si>
+    <t>0.10112743</t>
+  </si>
+  <si>
+    <t>0.9031137</t>
+  </si>
+  <si>
+    <t>0.10283567</t>
+  </si>
+  <si>
+    <t>0.9047731</t>
+  </si>
+  <si>
+    <t>0.9045251</t>
+  </si>
+  <si>
+    <t>0.9049966</t>
+  </si>
+  <si>
+    <t>0.9045735</t>
+  </si>
+  <si>
+    <t>0.10198155</t>
+  </si>
+  <si>
+    <t>0.9051515</t>
+  </si>
+  <si>
+    <t>0.9049999</t>
+  </si>
+  <si>
+    <t>0.9058942</t>
+  </si>
+  <si>
+    <t>0.9069242</t>
+  </si>
+  <si>
+    <t>0.9043745</t>
+  </si>
+  <si>
+    <t>0.9125512</t>
+  </si>
+  <si>
+    <t>0.9144808</t>
+  </si>
+  <si>
+    <t>0.9146701</t>
+  </si>
+  <si>
+    <t>0.9141422</t>
+  </si>
+  <si>
+    <t>0.9142923</t>
+  </si>
+  <si>
+    <t>0.9149038</t>
+  </si>
+  <si>
+    <t>0.10232320</t>
+  </si>
+  <si>
+    <t>0.9150995</t>
+  </si>
+  <si>
+    <t>0.9150332</t>
+  </si>
+  <si>
+    <t>0.9150318</t>
+  </si>
+  <si>
+    <t>0.9136061</t>
+  </si>
+  <si>
+    <t>0.10403143</t>
+  </si>
+  <si>
+    <t>0.10761872</t>
+  </si>
+  <si>
+    <t>0.9134406</t>
+  </si>
+  <si>
+    <t>0.10796037</t>
+  </si>
+  <si>
+    <t>0.9150258</t>
+  </si>
+  <si>
+    <t>0.10727708</t>
+  </si>
+  <si>
+    <t>0.9142720</t>
+  </si>
+  <si>
+    <t>0.9149173</t>
+  </si>
+  <si>
+    <t>0.10744790</t>
+  </si>
+  <si>
+    <t>0.9140457</t>
+  </si>
+  <si>
+    <t>0.9139981</t>
+  </si>
+  <si>
+    <t>0.9149645</t>
+  </si>
+  <si>
+    <t>0.9148137</t>
+  </si>
+  <si>
+    <t>0.10642296</t>
+  </si>
+  <si>
+    <t>0.9149001</t>
+  </si>
+  <si>
+    <t>0.10915613</t>
+  </si>
+  <si>
+    <t>0.9137677</t>
+  </si>
+  <si>
+    <t>0.10898531</t>
+  </si>
+  <si>
+    <t>0.9016746</t>
+  </si>
+  <si>
+    <t>0.9038273</t>
+  </si>
+  <si>
+    <t>0.9040292</t>
+  </si>
+  <si>
+    <t>0.10932696</t>
+  </si>
+  <si>
+    <t>0.9036264</t>
+  </si>
+  <si>
+    <t>0.10693543</t>
+  </si>
+  <si>
+    <t>0.9039946</t>
+  </si>
+  <si>
+    <t>0.10676461</t>
+  </si>
+  <si>
+    <t>0.9041767</t>
+  </si>
+  <si>
+    <t>0.10437308</t>
+  </si>
+  <si>
+    <t>0.9037996</t>
+  </si>
+  <si>
+    <t>0.9042967</t>
+  </si>
+  <si>
+    <t>0.9037429</t>
   </si>
   <si>
     <t>0.10573967</t>
   </si>
   <si>
-    <t>0.9148245</t>
-  </si>
-  <si>
-    <t>0.10454390</t>
-  </si>
-  <si>
-    <t>0.9146726</t>
-  </si>
-  <si>
-    <t>0.10796037</t>
-  </si>
-  <si>
-    <t>0.9132757</t>
-  </si>
-  <si>
-    <t>0.10522720</t>
-  </si>
-  <si>
-    <t>0.9127031</t>
-  </si>
-  <si>
-    <t>0.9142132</t>
-  </si>
-  <si>
-    <t>0.10676461</t>
-  </si>
-  <si>
-    <t>0.9138763</t>
-  </si>
-  <si>
-    <t>0.10625214</t>
-  </si>
-  <si>
-    <t>0.9145978</t>
-  </si>
-  <si>
-    <t>0.10659378</t>
-  </si>
-  <si>
-    <t>0.9138904</t>
-  </si>
-  <si>
-    <t>0.10642296</t>
-  </si>
-  <si>
-    <t>0.9138174</t>
-  </si>
-  <si>
-    <t>0.10608131</t>
-  </si>
-  <si>
-    <t>0.9038205</t>
-  </si>
-  <si>
-    <t>0.9059547</t>
-  </si>
-  <si>
-    <t>0.9053673</t>
-  </si>
-  <si>
-    <t>0.10813119</t>
-  </si>
-  <si>
-    <t>0.9038757</t>
-  </si>
-  <si>
-    <t>0.9050232</t>
-  </si>
-  <si>
-    <t>0.10437308</t>
-  </si>
-  <si>
-    <t>0.9055370</t>
-  </si>
-  <si>
-    <t>0.10403143</t>
-  </si>
-  <si>
-    <t>0.9057737</t>
-  </si>
-  <si>
-    <t>0.10386061</t>
-  </si>
-  <si>
-    <t>0.9057217</t>
-  </si>
-  <si>
-    <t>0.10471472</t>
-  </si>
-  <si>
-    <t>0.9050954</t>
-  </si>
-  <si>
-    <t>0.10539802</t>
-  </si>
-  <si>
-    <t>0.9057504</t>
+    <t>0.9044239</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,6 +511,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,8 +543,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +994,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -894,10 +1005,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -905,10 +1016,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -916,10 +1027,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -927,10 +1038,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -938,10 +1049,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
@@ -949,10 +1060,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
@@ -963,7 +1074,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -971,10 +1082,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -982,10 +1093,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
@@ -993,10 +1104,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -1004,10 +1115,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -1015,10 +1126,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1026,10 +1137,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1037,10 +1148,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1048,10 +1159,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -1059,10 +1170,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1070,10 +1181,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1081,10 +1192,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1092,10 +1203,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
         <v>67</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1103,10 +1214,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
         <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
@@ -1114,10 +1225,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>24</v>
@@ -1125,10 +1236,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>24</v>
@@ -1136,10 +1247,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
@@ -1147,10 +1258,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>76</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
@@ -1158,10 +1269,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1169,10 +1280,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>24</v>
@@ -1180,10 +1291,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>24</v>
@@ -1191,10 +1302,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
         <v>24</v>
@@ -1202,10 +1313,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
         <v>24</v>
@@ -1221,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C725FB-0259-044F-8EEE-299F54C2EEBC}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A32" zoomScale="81" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1350,10 +1461,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1361,10 +1472,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -1372,10 +1483,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -1383,10 +1494,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -1394,10 +1505,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -1405,10 +1516,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
@@ -1416,10 +1527,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
@@ -1430,7 +1541,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1438,10 +1549,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>46</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
@@ -1449,10 +1560,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
@@ -1460,10 +1571,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" t="s">
-        <v>51</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -1471,10 +1582,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -1482,10 +1593,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
         <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1493,10 +1604,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
         <v>56</v>
-      </c>
-      <c r="B25" t="s">
-        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1504,10 +1615,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
         <v>58</v>
-      </c>
-      <c r="B26" t="s">
-        <v>59</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1515,10 +1626,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
         <v>60</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -1526,10 +1637,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
         <v>62</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1537,10 +1648,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1548,10 +1659,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1559,10 +1670,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
         <v>67</v>
-      </c>
-      <c r="B31" t="s">
-        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1570,10 +1681,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
         <v>69</v>
-      </c>
-      <c r="B32" t="s">
-        <v>70</v>
       </c>
       <c r="C32" t="s">
         <v>24</v>
@@ -1581,10 +1692,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>24</v>
@@ -1592,10 +1703,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>73</v>
       </c>
       <c r="C34" t="s">
         <v>24</v>
@@ -1603,10 +1714,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35" t="s">
         <v>24</v>
@@ -1614,10 +1725,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
         <v>75</v>
-      </c>
-      <c r="B36" t="s">
-        <v>76</v>
       </c>
       <c r="C36" t="s">
         <v>24</v>
@@ -1625,10 +1736,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1636,10 +1747,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>79</v>
       </c>
       <c r="C38" t="s">
         <v>24</v>
@@ -1647,10 +1758,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
         <v>24</v>
@@ -1658,10 +1769,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
         <v>24</v>
@@ -1669,10 +1780,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
         <v>24</v>
@@ -1680,120 +1791,120 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C52" t="s">
         <v>25</v>
@@ -1801,10 +1912,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C53" t="s">
         <v>25</v>
@@ -1812,10 +1923,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="s">
         <v>100</v>
-      </c>
-      <c r="B54" t="s">
-        <v>105</v>
       </c>
       <c r="C54" t="s">
         <v>25</v>
@@ -1823,10 +1934,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
         <v>25</v>
@@ -1834,10 +1945,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C56" t="s">
         <v>25</v>
@@ -1845,10 +1956,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
         <v>25</v>
@@ -1856,10 +1967,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
         <v>25</v>
@@ -1867,10 +1978,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C59" t="s">
         <v>25</v>
@@ -1878,10 +1989,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>25</v>
@@ -1889,13 +2000,920 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE70A919-51A8-384A-AAAE-82A240E9E1DE}">
+  <dimension ref="A1:C81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>86</v>
+      </c>
+      <c r="B67" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>86</v>
+      </c>
+      <c r="B68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>133</v>
+      </c>
+      <c r="B70" t="s">
+        <v>134</v>
+      </c>
+      <c r="C70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>135</v>
+      </c>
+      <c r="B71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>137</v>
+      </c>
+      <c r="B72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>143</v>
+      </c>
+      <c r="B76" t="s">
+        <v>144</v>
+      </c>
+      <c r="C76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>149</v>
+      </c>
+      <c r="C79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>120</v>
+      </c>
+      <c r="B80" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>151</v>
+      </c>
+      <c r="B81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C81" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incluyendo Python en el documento
</commit_message>
<xml_diff>
--- a/ComparativaModelos.xlsx
+++ b/ComparativaModelos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/UCM/Machine Learning/Practica ML/MachineLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFDE973-CC26-5A46-AF05-0091F290C6A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6854F944-EE7E-1747-9694-4EC91DED3573}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="-18080" windowWidth="28800" windowHeight="16340" activeTab="5" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
+    <workbookView xWindow="8540" yWindow="-18100" windowWidth="28800" windowHeight="16340" activeTab="7" xr2:uid="{F64FD7D0-F0DF-1E4D-8389-72ADA7B6EEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="avnnet" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="svm" sheetId="5" r:id="rId5"/>
     <sheet name="xgboost" sheetId="6" r:id="rId6"/>
     <sheet name="ensamblado" sheetId="7" r:id="rId7"/>
+    <sheet name="python_vs_r" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2295" uniqueCount="477">
   <si>
     <t>tasa</t>
   </si>
@@ -1399,13 +1400,85 @@
   </si>
   <si>
     <t>XGBOOST</t>
+  </si>
+  <si>
+    <t>RANDOM FOREST</t>
+  </si>
+  <si>
+    <t>lenguaje</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>0.892160688365066</t>
+  </si>
+  <si>
+    <t>0.890580041956979</t>
+  </si>
+  <si>
+    <t>0.892536685185839</t>
+  </si>
+  <si>
+    <t>0.893679847761666</t>
+  </si>
+  <si>
+    <t>0.893196129621607</t>
+  </si>
+  <si>
+    <t>0.893341275043048</t>
+  </si>
+  <si>
+    <t>0.893676135720543</t>
+  </si>
+  <si>
+    <t>0.89239223493023</t>
+  </si>
+  <si>
+    <t>0.891011368909</t>
+  </si>
+  <si>
+    <t>0.892912647441903</t>
+  </si>
+  <si>
+    <t>0.900811921744751</t>
+  </si>
+  <si>
+    <t>0.900504056679263</t>
+  </si>
+  <si>
+    <t>0.900810626500151</t>
+  </si>
+  <si>
+    <t>0.903456495906542</t>
+  </si>
+  <si>
+    <t>0.902461181942952</t>
+  </si>
+  <si>
+    <t>0.901750442533506</t>
+  </si>
+  <si>
+    <t>0.902829119238763</t>
+  </si>
+  <si>
+    <t>0.901677951931684</t>
+  </si>
+  <si>
+    <t>0.904192897776748</t>
+  </si>
+  <si>
+    <t>0.902127005416476</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1425,6 +1498,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1447,9 +1533,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6744,8 +6832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E5D001-6A79-E343-8C9E-36C8C0394D2C}">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD81"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C41" sqref="B32:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7761,7 +7849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165A9ECD-B3AF-2A4D-B299-10A726DE42FC}">
   <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
@@ -9749,4 +9837,563 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4359140-C14C-CE41-B480-6A8020A8BEA2}">
+  <dimension ref="A1:N57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B2" t="s">
+        <v>453</v>
+      </c>
+      <c r="C2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B4" t="s">
+        <v>453</v>
+      </c>
+      <c r="C4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B6" t="s">
+        <v>453</v>
+      </c>
+      <c r="C6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>461</v>
+      </c>
+      <c r="B7" t="s">
+        <v>453</v>
+      </c>
+      <c r="C7" t="s">
+        <v>455</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8" t="s">
+        <v>455</v>
+      </c>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>463</v>
+      </c>
+      <c r="B9" t="s">
+        <v>453</v>
+      </c>
+      <c r="C9" t="s">
+        <v>455</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>464</v>
+      </c>
+      <c r="B10" t="s">
+        <v>453</v>
+      </c>
+      <c r="C10" t="s">
+        <v>455</v>
+      </c>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>465</v>
+      </c>
+      <c r="B11" t="s">
+        <v>453</v>
+      </c>
+      <c r="C11" t="s">
+        <v>455</v>
+      </c>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>466</v>
+      </c>
+      <c r="B12" t="s">
+        <v>452</v>
+      </c>
+      <c r="C12" t="s">
+        <v>455</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>467</v>
+      </c>
+      <c r="B13" t="s">
+        <v>452</v>
+      </c>
+      <c r="C13" t="s">
+        <v>455</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>468</v>
+      </c>
+      <c r="B14" t="s">
+        <v>452</v>
+      </c>
+      <c r="C14" t="s">
+        <v>455</v>
+      </c>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>469</v>
+      </c>
+      <c r="B15" t="s">
+        <v>452</v>
+      </c>
+      <c r="C15" t="s">
+        <v>455</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>470</v>
+      </c>
+      <c r="B16" t="s">
+        <v>452</v>
+      </c>
+      <c r="C16" t="s">
+        <v>455</v>
+      </c>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>471</v>
+      </c>
+      <c r="B17" t="s">
+        <v>452</v>
+      </c>
+      <c r="C17" t="s">
+        <v>455</v>
+      </c>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>472</v>
+      </c>
+      <c r="B18" t="s">
+        <v>452</v>
+      </c>
+      <c r="C18" t="s">
+        <v>455</v>
+      </c>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>473</v>
+      </c>
+      <c r="B19" t="s">
+        <v>452</v>
+      </c>
+      <c r="C19" t="s">
+        <v>455</v>
+      </c>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>474</v>
+      </c>
+      <c r="B20" t="s">
+        <v>452</v>
+      </c>
+      <c r="C20" t="s">
+        <v>455</v>
+      </c>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>475</v>
+      </c>
+      <c r="B21" t="s">
+        <v>452</v>
+      </c>
+      <c r="C21" t="s">
+        <v>455</v>
+      </c>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>453</v>
+      </c>
+      <c r="C22" t="s">
+        <v>476</v>
+      </c>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" t="s">
+        <v>453</v>
+      </c>
+      <c r="C23" t="s">
+        <v>476</v>
+      </c>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24" t="s">
+        <v>476</v>
+      </c>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" t="s">
+        <v>453</v>
+      </c>
+      <c r="C25" t="s">
+        <v>476</v>
+      </c>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
+        <v>453</v>
+      </c>
+      <c r="C26" t="s">
+        <v>476</v>
+      </c>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" t="s">
+        <v>453</v>
+      </c>
+      <c r="C27" t="s">
+        <v>476</v>
+      </c>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
+        <v>453</v>
+      </c>
+      <c r="C28" t="s">
+        <v>476</v>
+      </c>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" t="s">
+        <v>476</v>
+      </c>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" t="s">
+        <v>453</v>
+      </c>
+      <c r="C30" t="s">
+        <v>476</v>
+      </c>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" t="s">
+        <v>453</v>
+      </c>
+      <c r="C31" t="s">
+        <v>476</v>
+      </c>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>437</v>
+      </c>
+      <c r="B32" t="s">
+        <v>452</v>
+      </c>
+      <c r="C32" t="s">
+        <v>476</v>
+      </c>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>439</v>
+      </c>
+      <c r="B33" t="s">
+        <v>452</v>
+      </c>
+      <c r="C33" t="s">
+        <v>476</v>
+      </c>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>441</v>
+      </c>
+      <c r="B34" t="s">
+        <v>452</v>
+      </c>
+      <c r="C34" t="s">
+        <v>476</v>
+      </c>
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" t="s">
+        <v>452</v>
+      </c>
+      <c r="C35" t="s">
+        <v>476</v>
+      </c>
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>443</v>
+      </c>
+      <c r="B36" t="s">
+        <v>452</v>
+      </c>
+      <c r="C36" t="s">
+        <v>476</v>
+      </c>
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>445</v>
+      </c>
+      <c r="B37" t="s">
+        <v>452</v>
+      </c>
+      <c r="C37" t="s">
+        <v>476</v>
+      </c>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>447</v>
+      </c>
+      <c r="B38" t="s">
+        <v>452</v>
+      </c>
+      <c r="C38" t="s">
+        <v>476</v>
+      </c>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>449</v>
+      </c>
+      <c r="B39" t="s">
+        <v>452</v>
+      </c>
+      <c r="C39" t="s">
+        <v>476</v>
+      </c>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>450</v>
+      </c>
+      <c r="B40" t="s">
+        <v>452</v>
+      </c>
+      <c r="C40" t="s">
+        <v>476</v>
+      </c>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>451</v>
+      </c>
+      <c r="B41" t="s">
+        <v>452</v>
+      </c>
+      <c r="C41" t="s">
+        <v>476</v>
+      </c>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="N44" s="3"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="N45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="N46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N48" s="3"/>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N49" s="3"/>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N50" s="3"/>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N51" s="3"/>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N52" s="3"/>
+    </row>
+    <row r="53" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N53" s="3"/>
+    </row>
+    <row r="54" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N54" s="3"/>
+    </row>
+    <row r="55" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N55" s="3"/>
+    </row>
+    <row r="56" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N56" s="3"/>
+    </row>
+    <row r="57" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N57" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>